<commit_message>
Update Summary and BOM
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Pull-Tab_Tin_Can_Opener_BOM.xlsx
+++ b/Documentation/Working_Documents/Pull-Tab_Tin_Can_Opener_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-Team/Shared Documents/Server/3 AT Library/WIP/Can Openers/Pull-Tab_Tin_Can_Opener/GitHub/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FCBEFA0-6D7D-4B40-AE8B-DFFD68EE726B}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2217FAC2-592C-4F13-A922-007303180590}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
     <t>The single part for the full functional can opener.</t>
   </si>
   <si>
-    <t>Add github link</t>
+    <t>https://github.com/makersmakingchange/Pull-Tab-Tin-Can-Opener</t>
   </si>
 </sst>
 </file>
@@ -112,7 +112,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,15 +186,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -345,7 +336,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1"/>
@@ -371,7 +362,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
@@ -659,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,7 +757,7 @@
       <c r="F5">
         <v>122</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -783,20 +773,21 @@
       <c r="G6" s="11"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{E9B2FD16-BB6B-4936-A91D-81A9DBE66EE2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1037,21 +1028,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
-    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1076,9 +1066,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
+    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Update Summary and BOM"
This reverts commit bc97cbde53706c8a9a4818ee2694dbdf19bd6d33.
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Pull-Tab_Tin_Can_Opener_BOM.xlsx
+++ b/Documentation/Working_Documents/Pull-Tab_Tin_Can_Opener_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-Team/Shared Documents/Server/3 AT Library/WIP/Can Openers/Pull-Tab_Tin_Can_Opener/GitHub/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2217FAC2-592C-4F13-A922-007303180590}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FCBEFA0-6D7D-4B40-AE8B-DFFD68EE726B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
     <t>The single part for the full functional can opener.</t>
   </si>
   <si>
-    <t>https://github.com/makersmakingchange/Pull-Tab-Tin-Can-Opener</t>
+    <t>Add github link</t>
   </si>
 </sst>
 </file>
@@ -112,7 +112,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +186,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -336,7 +345,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1"/>
@@ -362,6 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
@@ -649,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,7 +767,7 @@
       <c r="F5">
         <v>122</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="23" t="s">
         <v>17</v>
       </c>
     </row>
@@ -773,21 +783,20 @@
       <c r="G6" s="11"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{E9B2FD16-BB6B-4936-A91D-81A9DBE66EE2}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1028,20 +1037,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
+    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1066,12 +1076,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
-    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update BOM and Summary 2
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Pull-Tab_Tin_Can_Opener_BOM.xlsx
+++ b/Documentation/Working_Documents/Pull-Tab_Tin_Can_Opener_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-Team/Shared Documents/Server/3 AT Library/WIP/Can Openers/Pull-Tab_Tin_Can_Opener/GitHub/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FCBEFA0-6D7D-4B40-AE8B-DFFD68EE726B}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2217FAC2-592C-4F13-A922-007303180590}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
     <t>The single part for the full functional can opener.</t>
   </si>
   <si>
-    <t>Add github link</t>
+    <t>https://github.com/makersmakingchange/Pull-Tab-Tin-Can-Opener</t>
   </si>
 </sst>
 </file>
@@ -112,7 +112,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,15 +186,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -345,7 +336,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1"/>
@@ -371,7 +362,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
@@ -659,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,7 +757,7 @@
       <c r="F5">
         <v>122</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -783,20 +773,21 @@
       <c r="G6" s="11"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{E9B2FD16-BB6B-4936-A91D-81A9DBE66EE2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1037,21 +1028,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
-    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1076,9 +1066,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
+    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Edits to Summary, BOM, User Guide, Maker Checklist
</commit_message>
<xml_diff>
--- a/Documentation/Working_Documents/Pull-Tab_Tin_Can_Opener_BOM.xlsx
+++ b/Documentation/Working_Documents/Pull-Tab_Tin_Can_Opener_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://neilsquiresoc.sharepoint.com/sites/MMC-Team/Shared Documents/Server/3 AT Library/WIP/Can Openers/Pull-Tab_Tin_Can_Opener/GitHub/Documentation/Working_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2217FAC2-592C-4F13-A922-007303180590}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_DC0E2523FAFE28515E8D5C5A1D4A6B02C3B15AFA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7EBFBB2-01AA-460D-8EFB-F71F3FB78E05}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Total Cost</t>
   </si>
@@ -62,9 +62,33 @@
     </r>
   </si>
   <si>
+    <t>Date Created: 4/20/2021</t>
+  </si>
+  <si>
+    <t>Commercial Parts:</t>
+  </si>
+  <si>
+    <t>Part type (Electrical. Mechanical, Sanitization, ect)</t>
+  </si>
+  <si>
+    <t>Part Name</t>
+  </si>
+  <si>
     <t>Quantity Needed</t>
   </si>
   <si>
+    <t>Pkg Quantity</t>
+  </si>
+  <si>
+    <t>Price per package</t>
+  </si>
+  <si>
+    <t>Price per Unit</t>
+  </si>
+  <si>
+    <t>Price for qty needed</t>
+  </si>
+  <si>
     <t>Link</t>
   </si>
   <si>
@@ -89,10 +113,19 @@
     <t>Total Print Cost:</t>
   </si>
   <si>
+    <t>Tools for Assembly</t>
+  </si>
+  <si>
+    <t>Alternatives (if there are other sources for some parts link them below)</t>
+  </si>
+  <si>
+    <t>Part and description</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>Device: Pull-Tab Tin Can Opener</t>
-  </si>
-  <si>
-    <t>Date Created: 6/20/2022</t>
   </si>
   <si>
     <t>Pull-Tab_Tin_Can_Opener.stl</t>
@@ -112,7 +145,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +198,14 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -187,7 +228,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,18 +265,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -259,6 +294,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -270,6 +331,15 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -277,52 +347,74 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -336,7 +428,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1"/>
@@ -346,22 +438,28 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="9" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Accent4" xfId="3" builtinId="44"/>
@@ -647,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -668,9 +766,9 @@
     <col min="12" max="12" width="89.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" ht="36" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -682,99 +780,201 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>14</v>
+      <c r="B2" s="11" t="s">
+        <v>4</v>
       </c>
       <c r="C2" s="5">
-        <f>SUM(G3:G3)+E6</f>
+        <f>SUM(G5:G7)+E10</f>
         <v>0.5</v>
       </c>
       <c r="D2" s="18">
-        <f>SUM(F5:F5)/60</f>
+        <f>SUM(F9:F9)/60</f>
         <v>2.0333333333333332</v>
       </c>
       <c r="E2" s="6">
-        <f>SUM(D5:D5)</f>
+        <f>SUM(D9:D9)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="21">
-        <v>25</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="L3" s="8"/>
+    <row r="3" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="21"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="22">
+        <v>25</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="26"/>
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
+      <c r="C8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D9">
         <v>20</v>
       </c>
-      <c r="E5" s="14">
-        <f>(D5/1000)*$B$3</f>
+      <c r="E9" s="28">
+        <f>(D9/1000)*$B$7</f>
         <v>0.5</v>
       </c>
-      <c r="F5">
+      <c r="F9">
         <v>122</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="D6" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="16">
-        <f>SUM(E5:E5)</f>
+      <c r="G9" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11"/>
+      <c r="D10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="17">
+        <f>SUM(E9:E9)</f>
         <v>0.5</v>
       </c>
-      <c r="G6" s="11"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" xr:uid="{E9B2FD16-BB6B-4936-A91D-81A9DBE66EE2}"/>
+    <hyperlink ref="G9" r:id="rId1" xr:uid="{47297394-1504-4293-99DE-9EC195EDF1E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -791,6 +991,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100456CAEA290209545A9F8681F83603874" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d27786a72e09a52c769a64d5f7eeaa24">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8cf100d1-0775-4feb-8634-62999c4541bc" xmlns:ns3="38b325e6-602c-452a-8617-173bf47082c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03ae89856d271009074f70b56337b48d" ns2:_="" ns3:_="">
     <xsd:import namespace="8cf100d1-0775-4feb-8634-62999c4541bc"/>
@@ -1027,17 +1238,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="38b325e6-602c-452a-8617-173bf47082c5" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8cf100d1-0775-4feb-8634-62999c4541bc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4740145F-09D2-466B-B9A2-2798696B0ADF}">
   <ds:schemaRefs>
@@ -1047,6 +1247,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
+    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99BECD52-63A8-454F-82E6-6195B786F95C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1063,15 +1274,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4958292-C6C4-482B-887A-6CF9FB19AB74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38b325e6-602c-452a-8617-173bf47082c5"/>
-    <ds:schemaRef ds:uri="8cf100d1-0775-4feb-8634-62999c4541bc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>